<commit_message>
Country moved from OrderProduct to Order
</commit_message>
<xml_diff>
--- a/storage/app/excel/templates/order-products.xlsx
+++ b/storage/app/excel/templates/order-products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSPanel\home\business-processes2\storage\app\excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9E1CED-C11A-4C8F-BA21-C3638F873EDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53736B2-749D-4560-BF85-EA961AB8A739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -480,7 +480,7 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +517,7 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G1" s="4" t="s">

</xml_diff>